<commit_message>
Prev BUR testing files were using more recent 2024 file that reflected some 2025 changes like 126 EE that moved from IPS to different segments. Reran with frozen 2024 file. Need to address where to use ytd_annualized vs. just ytd. potentially will change ytd_value or FY commit/forcast number
</commit_message>
<xml_diff>
--- a/outputs/BURs/BUR Testing_AMC.xlsx
+++ b/outputs/BURs/BUR Testing_AMC.xlsx
@@ -96,7 +96,7 @@
     <t xml:space="preserve">AMC Aerospace Solutions Division</t>
   </si>
   <si>
-    <t xml:space="preserve">Voluntary Turnover Professional</t>
+    <t xml:space="preserve">Professional Voluntary Turnover</t>
   </si>
   <si>
     <t xml:space="preserve">PY Actual</t>
@@ -589,13 +589,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.0228</v>
+        <v>0.0229</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>0.0324</v>
+        <v>0.0326</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0.018</v>
+        <v>0.0181</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>0.0045</v>
@@ -604,7 +604,7 @@
         <v>0.0132</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0.0356</v>
+        <v>0.0357</v>
       </c>
       <c r="N2" s="1" t="n">
         <v>0.0043</v>
@@ -616,10 +616,10 @@
         <v>0.0167</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>0.0299</v>
+        <v>0.0298</v>
       </c>
       <c r="R2" s="1" t="n">
-        <v>0.0163</v>
+        <v>0.0162</v>
       </c>
       <c r="S2" s="1" t="n">
         <v>0</v>
@@ -628,10 +628,10 @@
         <v>0.0039</v>
       </c>
       <c r="U2" s="1" t="n">
-        <v>0.0199</v>
+        <v>0.0198</v>
       </c>
       <c r="V2" s="1" t="n">
-        <v>0.1166</v>
+        <v>0.1165</v>
       </c>
     </row>
     <row r="3">
@@ -657,13 +657,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>0.02052</v>
+        <v>0.02061</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>0.02916</v>
+        <v>0.02934</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>0.0162</v>
+        <v>0.01629</v>
       </c>
       <c r="K3" s="1" t="n">
         <v>0.00405</v>
@@ -672,7 +672,7 @@
         <v>0.01188</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>0.03204</v>
+        <v>0.03213</v>
       </c>
       <c r="N3" s="1" t="n">
         <v>0.00387</v>
@@ -684,10 +684,10 @@
         <v>0.01503</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>0.02691</v>
+        <v>0.02682</v>
       </c>
       <c r="R3" s="1" t="n">
-        <v>0.01467</v>
+        <v>0.01458</v>
       </c>
       <c r="S3" s="1" t="n">
         <v>0</v>
@@ -696,10 +696,10 @@
         <v>0.00351</v>
       </c>
       <c r="U3" s="1" t="n">
-        <v>0.01791</v>
+        <v>0.01782</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>0.10494</v>
+        <v>0.10485</v>
       </c>
     </row>
     <row r="4">
@@ -740,7 +740,7 @@
         <v>0.01245</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.03735</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>0.01245</v>
@@ -752,7 +752,7 @@
         <v>0.01245</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.03735</v>
       </c>
       <c r="R4" s="1" t="n">
         <v>0.01245</v>
@@ -764,7 +764,7 @@
         <v>0.01245</v>
       </c>
       <c r="U4" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.03735</v>
       </c>
       <c r="V4" s="1" t="n">
         <v>0.1494</v>
@@ -1097,31 +1097,31 @@
         <v>0</v>
       </c>
       <c r="N2" s="10" t="n">
-        <v>0.0141</v>
+        <v>0.0139</v>
       </c>
       <c r="O2" s="10" t="n">
-        <v>0.0303</v>
+        <v>0.0299</v>
       </c>
       <c r="P2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="Q2" s="10" t="n">
-        <v>0.0441</v>
+        <v>0.0435</v>
       </c>
       <c r="R2" s="10" t="n">
-        <v>0.0149</v>
+        <v>0.0147</v>
       </c>
       <c r="S2" s="10" t="n">
-        <v>0.0154</v>
+        <v>0.0152</v>
       </c>
       <c r="T2" s="10" t="n">
-        <v>0.0312</v>
+        <v>0.0308</v>
       </c>
       <c r="U2" s="10" t="n">
-        <v>0.0613</v>
+        <v>0.0603</v>
       </c>
       <c r="V2" s="10" t="n">
-        <v>0.1045</v>
+        <v>0.1029</v>
       </c>
     </row>
     <row r="3">
@@ -1165,31 +1165,31 @@
         <v>0</v>
       </c>
       <c r="N3" s="10" t="n">
-        <v>0.01269</v>
+        <v>0.01251</v>
       </c>
       <c r="O3" s="10" t="n">
-        <v>0.02727</v>
+        <v>0.02691</v>
       </c>
       <c r="P3" s="10" t="n">
         <v>0</v>
       </c>
       <c r="Q3" s="10" t="n">
-        <v>0.03969</v>
+        <v>0.03915</v>
       </c>
       <c r="R3" s="10" t="n">
-        <v>0.01341</v>
+        <v>0.01323</v>
       </c>
       <c r="S3" s="10" t="n">
-        <v>0.01386</v>
+        <v>0.01368</v>
       </c>
       <c r="T3" s="10" t="n">
-        <v>0.02808</v>
+        <v>0.02772</v>
       </c>
       <c r="U3" s="10" t="n">
-        <v>0.05517</v>
+        <v>0.05427</v>
       </c>
       <c r="V3" s="10" t="n">
-        <v>0.09405</v>
+        <v>0.09261</v>
       </c>
     </row>
     <row r="4">
@@ -1230,7 +1230,7 @@
         <v>0.25</v>
       </c>
       <c r="M4" s="10" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="N4" s="10" t="n">
         <v>0.25</v>
@@ -1242,7 +1242,7 @@
         <v>0.25</v>
       </c>
       <c r="Q4" s="10" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="R4" s="10" t="n">
         <v>0.25</v>
@@ -1254,7 +1254,7 @@
         <v>0.25</v>
       </c>
       <c r="U4" s="10" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="V4" s="10" t="n">
         <v>3</v>
@@ -1479,55 +1479,55 @@
         <v>25</v>
       </c>
       <c r="F2" s="11" t="n">
-        <v>0.0073</v>
+        <v>0.0076</v>
       </c>
       <c r="G2" s="11" t="n">
-        <v>0.0055</v>
+        <v>0.0057</v>
       </c>
       <c r="H2" s="11" t="n">
-        <v>0.0084</v>
+        <v>0.0091</v>
       </c>
       <c r="I2" s="11" t="n">
-        <v>0.0212</v>
+        <v>0.0224</v>
       </c>
       <c r="J2" s="11" t="n">
-        <v>0.0088</v>
+        <v>0.0092</v>
       </c>
       <c r="K2" s="11" t="n">
-        <v>0.0103</v>
+        <v>0.0107</v>
       </c>
       <c r="L2" s="11" t="n">
-        <v>0.0077</v>
+        <v>0.008</v>
       </c>
       <c r="M2" s="11" t="n">
-        <v>0.0268</v>
+        <v>0.0279</v>
       </c>
       <c r="N2" s="11" t="n">
-        <v>0.0067</v>
+        <v>0.007</v>
       </c>
       <c r="O2" s="11" t="n">
-        <v>0.0109</v>
+        <v>0.0114</v>
       </c>
       <c r="P2" s="11" t="n">
-        <v>0.0102</v>
+        <v>0.0106</v>
       </c>
       <c r="Q2" s="11" t="n">
-        <v>0.0277</v>
+        <v>0.0289</v>
       </c>
       <c r="R2" s="11" t="n">
-        <v>0.0083</v>
+        <v>0.009</v>
       </c>
       <c r="S2" s="11" t="n">
-        <v>0.0072</v>
+        <v>0.0075</v>
       </c>
       <c r="T2" s="11" t="n">
         <v>0.0094</v>
       </c>
       <c r="U2" s="11" t="n">
-        <v>0.0249</v>
+        <v>0.026</v>
       </c>
       <c r="V2" s="11" t="n">
-        <v>0.1005</v>
+        <v>0.1051</v>
       </c>
     </row>
     <row r="3">
@@ -1547,55 +1547,55 @@
         <v>26</v>
       </c>
       <c r="F3" s="11" t="n">
-        <v>0.00657</v>
+        <v>0.00684</v>
       </c>
       <c r="G3" s="11" t="n">
-        <v>0.00495</v>
+        <v>0.00513</v>
       </c>
       <c r="H3" s="11" t="n">
-        <v>0.00756</v>
+        <v>0.00819</v>
       </c>
       <c r="I3" s="11" t="n">
-        <v>0.01908</v>
+        <v>0.02016</v>
       </c>
       <c r="J3" s="11" t="n">
-        <v>0.00792</v>
+        <v>0.00828</v>
       </c>
       <c r="K3" s="11" t="n">
-        <v>0.00927</v>
+        <v>0.00963</v>
       </c>
       <c r="L3" s="11" t="n">
-        <v>0.00693</v>
+        <v>0.0072</v>
       </c>
       <c r="M3" s="11" t="n">
-        <v>0.02412</v>
+        <v>0.02511</v>
       </c>
       <c r="N3" s="11" t="n">
-        <v>0.00603</v>
+        <v>0.0063</v>
       </c>
       <c r="O3" s="11" t="n">
-        <v>0.00981</v>
+        <v>0.01026</v>
       </c>
       <c r="P3" s="11" t="n">
-        <v>0.00918</v>
+        <v>0.00954</v>
       </c>
       <c r="Q3" s="11" t="n">
-        <v>0.02493</v>
+        <v>0.02601</v>
       </c>
       <c r="R3" s="11" t="n">
-        <v>0.00747</v>
+        <v>0.0081</v>
       </c>
       <c r="S3" s="11" t="n">
-        <v>0.00648</v>
+        <v>0.00675</v>
       </c>
       <c r="T3" s="11" t="n">
         <v>0.00846</v>
       </c>
       <c r="U3" s="11" t="n">
-        <v>0.02241</v>
+        <v>0.0234</v>
       </c>
       <c r="V3" s="11" t="n">
-        <v>0.09045</v>
+        <v>0.09459</v>
       </c>
     </row>
     <row r="4">
@@ -1636,7 +1636,7 @@
         <v>0.00915</v>
       </c>
       <c r="M4" s="11" t="n">
-        <v>0.0366</v>
+        <v>0.02745</v>
       </c>
       <c r="N4" s="11" t="n">
         <v>0.00915</v>
@@ -1648,7 +1648,7 @@
         <v>0.00915</v>
       </c>
       <c r="Q4" s="11" t="n">
-        <v>0.0366</v>
+        <v>0.02745</v>
       </c>
       <c r="R4" s="11" t="n">
         <v>0.00915</v>
@@ -1660,7 +1660,7 @@
         <v>0.00915</v>
       </c>
       <c r="U4" s="11" t="n">
-        <v>0.0366</v>
+        <v>0.02745</v>
       </c>
       <c r="V4" s="11" t="n">
         <v>0.1098</v>
@@ -2319,55 +2319,55 @@
         <v>25</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0.0085</v>
+        <v>0.0097</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>0.0067</v>
+        <v>0.0077</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>0.0034</v>
+        <v>0.0058</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>0.0186</v>
+        <v>0.0232</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>0.0134</v>
+        <v>0.0154</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>0.0118</v>
+        <v>0.0136</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>0.0051</v>
+        <v>0.0059</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>0.0304</v>
+        <v>0.035</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>0.0052</v>
+        <v>0.0061</v>
       </c>
       <c r="O2" s="3" t="n">
-        <v>0.0142</v>
+        <v>0.0166</v>
       </c>
       <c r="P2" s="3" t="n">
-        <v>0.0179</v>
+        <v>0.0209</v>
       </c>
       <c r="Q2" s="3" t="n">
-        <v>0.0371</v>
+        <v>0.0432</v>
       </c>
       <c r="R2" s="3" t="n">
-        <v>0.0071</v>
+        <v>0.0083</v>
       </c>
       <c r="S2" s="3" t="n">
-        <v>0.0053</v>
+        <v>0.0063</v>
       </c>
       <c r="T2" s="3" t="n">
-        <v>0.0035</v>
+        <v>0.0041</v>
       </c>
       <c r="U2" s="3" t="n">
-        <v>0.016</v>
+        <v>0.0187</v>
       </c>
       <c r="V2" s="3" t="n">
-        <v>0.1021</v>
+        <v>0.1202</v>
       </c>
     </row>
     <row r="3">
@@ -2387,55 +2387,55 @@
         <v>26</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.00765</v>
+        <v>0.00873</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>0.00603</v>
+        <v>0.00693</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>0.00306</v>
+        <v>0.00522</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>0.01674</v>
+        <v>0.02088</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>0.01206</v>
+        <v>0.01386</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>0.01062</v>
+        <v>0.01224</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>0.00459</v>
+        <v>0.00531</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>0.02736</v>
+        <v>0.0315</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>0.00468</v>
+        <v>0.00549</v>
       </c>
       <c r="O3" s="3" t="n">
-        <v>0.01278</v>
+        <v>0.01494</v>
       </c>
       <c r="P3" s="3" t="n">
-        <v>0.01611</v>
+        <v>0.01881</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>0.03339</v>
+        <v>0.03888</v>
       </c>
       <c r="R3" s="3" t="n">
-        <v>0.00639</v>
+        <v>0.00747</v>
       </c>
       <c r="S3" s="3" t="n">
-        <v>0.00477</v>
+        <v>0.00567</v>
       </c>
       <c r="T3" s="3" t="n">
-        <v>0.00315</v>
+        <v>0.00369</v>
       </c>
       <c r="U3" s="3" t="n">
-        <v>0.0144</v>
+        <v>0.01683</v>
       </c>
       <c r="V3" s="3" t="n">
-        <v>0.09189</v>
+        <v>0.10818</v>
       </c>
     </row>
     <row r="4">
@@ -2476,7 +2476,7 @@
         <v>0.0111</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0.0444</v>
+        <v>0.0333</v>
       </c>
       <c r="N4" s="3" t="n">
         <v>0.0111</v>
@@ -2488,7 +2488,7 @@
         <v>0.0111</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>0.0444</v>
+        <v>0.0333</v>
       </c>
       <c r="R4" s="3" t="n">
         <v>0.0111</v>
@@ -2500,7 +2500,7 @@
         <v>0.0111</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>0.0444</v>
+        <v>0.0333</v>
       </c>
       <c r="V4" s="3" t="n">
         <v>0.1332</v>
@@ -2857,7 +2857,7 @@
         <v>0</v>
       </c>
       <c r="V2" s="4" t="n">
-        <v>0.1562</v>
+        <v>0.1587</v>
       </c>
     </row>
     <row r="3">
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="V3" s="4" t="n">
-        <v>0.14058</v>
+        <v>0.14283</v>
       </c>
     </row>
     <row r="4">
@@ -3199,55 +3199,55 @@
         <v>25</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>0.0102</v>
+        <v>0.0101</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>0.0041</v>
+        <v>0.004</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>0.0062</v>
+        <v>0.0061</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>0.0205</v>
+        <v>0.0203</v>
       </c>
       <c r="J2" s="5" t="n">
+        <v>0.0083</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="N2" s="5" t="n">
         <v>0.0084</v>
       </c>
-      <c r="K2" s="5" t="n">
-        <v>0.0148</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>0.0064</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>0.0296</v>
-      </c>
-      <c r="N2" s="5" t="n">
-        <v>0.0086</v>
-      </c>
       <c r="O2" s="5" t="n">
-        <v>0.0134</v>
+        <v>0.0132</v>
       </c>
       <c r="P2" s="5" t="n">
+        <v>0.0066</v>
+      </c>
+      <c r="Q2" s="5" t="n">
+        <v>0.0281</v>
+      </c>
+      <c r="R2" s="5" t="n">
+        <v>0.0111</v>
+      </c>
+      <c r="S2" s="5" t="n">
         <v>0.0067</v>
       </c>
-      <c r="Q2" s="5" t="n">
-        <v>0.0286</v>
-      </c>
-      <c r="R2" s="5" t="n">
-        <v>0.009</v>
-      </c>
-      <c r="S2" s="5" t="n">
-        <v>0.0068</v>
-      </c>
       <c r="T2" s="5" t="n">
-        <v>0.0091</v>
+        <v>0.0067</v>
       </c>
       <c r="U2" s="5" t="n">
-        <v>0.0249</v>
+        <v>0.0246</v>
       </c>
       <c r="V2" s="5" t="n">
-        <v>0.1034</v>
+        <v>0.102</v>
       </c>
     </row>
     <row r="3">
@@ -3267,55 +3267,55 @@
         <v>26</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.00918</v>
+        <v>0.00909</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>0.00369</v>
+        <v>0.0036</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>0.00558</v>
+        <v>0.00549</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>0.01845</v>
+        <v>0.01827</v>
       </c>
       <c r="J3" s="5" t="n">
+        <v>0.00747</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>0.01314</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0.00567</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>0.02628</v>
+      </c>
+      <c r="N3" s="5" t="n">
         <v>0.00756</v>
       </c>
-      <c r="K3" s="5" t="n">
-        <v>0.01332</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>0.00576</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>0.02664</v>
-      </c>
-      <c r="N3" s="5" t="n">
-        <v>0.00774</v>
-      </c>
       <c r="O3" s="5" t="n">
-        <v>0.01206</v>
+        <v>0.01188</v>
       </c>
       <c r="P3" s="5" t="n">
+        <v>0.00594</v>
+      </c>
+      <c r="Q3" s="5" t="n">
+        <v>0.02529</v>
+      </c>
+      <c r="R3" s="5" t="n">
+        <v>0.00999</v>
+      </c>
+      <c r="S3" s="5" t="n">
         <v>0.00603</v>
       </c>
-      <c r="Q3" s="5" t="n">
-        <v>0.02574</v>
-      </c>
-      <c r="R3" s="5" t="n">
-        <v>0.0081</v>
-      </c>
-      <c r="S3" s="5" t="n">
-        <v>0.00612</v>
-      </c>
       <c r="T3" s="5" t="n">
-        <v>0.00819</v>
+        <v>0.00603</v>
       </c>
       <c r="U3" s="5" t="n">
-        <v>0.02241</v>
+        <v>0.02214</v>
       </c>
       <c r="V3" s="5" t="n">
-        <v>0.09306</v>
+        <v>0.0918</v>
       </c>
     </row>
     <row r="4">
@@ -3356,7 +3356,7 @@
         <v>0.007675</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>0.0307</v>
+        <v>0.023025</v>
       </c>
       <c r="N4" s="5" t="n">
         <v>0.007675</v>
@@ -3368,7 +3368,7 @@
         <v>0.007675</v>
       </c>
       <c r="Q4" s="5" t="n">
-        <v>0.0307</v>
+        <v>0.023025</v>
       </c>
       <c r="R4" s="5" t="n">
         <v>0.007675</v>
@@ -3380,7 +3380,7 @@
         <v>0.007675</v>
       </c>
       <c r="U4" s="5" t="n">
-        <v>0.0307</v>
+        <v>0.023025</v>
       </c>
       <c r="V4" s="5" t="n">
         <v>0.0921</v>
@@ -3689,28 +3689,28 @@
         <v>25</v>
       </c>
       <c r="F2" s="6" t="n">
-        <v>0.0085</v>
+        <v>0.0086</v>
       </c>
       <c r="G2" s="6" t="n">
-        <v>0.0202</v>
+        <v>0.0203</v>
       </c>
       <c r="H2" s="6" t="n">
-        <v>0.0086</v>
+        <v>0.0087</v>
       </c>
       <c r="I2" s="6" t="n">
-        <v>0.0372</v>
+        <v>0.0376</v>
       </c>
       <c r="J2" s="6" t="n">
-        <v>0.0142</v>
+        <v>0.0144</v>
       </c>
       <c r="K2" s="6" t="n">
-        <v>0.0201</v>
+        <v>0.0203</v>
       </c>
       <c r="L2" s="6" t="n">
-        <v>0.0115</v>
+        <v>0.0116</v>
       </c>
       <c r="M2" s="6" t="n">
-        <v>0.0459</v>
+        <v>0.0463</v>
       </c>
       <c r="N2" s="6" t="n">
         <v>0.0085</v>
@@ -3722,22 +3722,22 @@
         <v>0.0028</v>
       </c>
       <c r="Q2" s="6" t="n">
-        <v>0.0195</v>
+        <v>0.0197</v>
       </c>
       <c r="R2" s="6" t="n">
-        <v>0.011</v>
+        <v>0.0111</v>
       </c>
       <c r="S2" s="6" t="n">
-        <v>0.0083</v>
+        <v>0.0084</v>
       </c>
       <c r="T2" s="6" t="n">
-        <v>0.0138</v>
+        <v>0.0139</v>
       </c>
       <c r="U2" s="6" t="n">
-        <v>0.0331</v>
+        <v>0.0333</v>
       </c>
       <c r="V2" s="6" t="n">
-        <v>0.1352</v>
+        <v>0.1364</v>
       </c>
     </row>
     <row r="3">
@@ -3757,28 +3757,28 @@
         <v>26</v>
       </c>
       <c r="F3" s="6" t="n">
-        <v>0.00765</v>
+        <v>0.00774</v>
       </c>
       <c r="G3" s="6" t="n">
-        <v>0.01818</v>
+        <v>0.01827</v>
       </c>
       <c r="H3" s="6" t="n">
-        <v>0.00774</v>
+        <v>0.00783</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>0.03348</v>
+        <v>0.03384</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>0.01278</v>
+        <v>0.01296</v>
       </c>
       <c r="K3" s="6" t="n">
-        <v>0.01809</v>
+        <v>0.01827</v>
       </c>
       <c r="L3" s="6" t="n">
-        <v>0.01035</v>
+        <v>0.01044</v>
       </c>
       <c r="M3" s="6" t="n">
-        <v>0.04131</v>
+        <v>0.04167</v>
       </c>
       <c r="N3" s="6" t="n">
         <v>0.00765</v>
@@ -3790,22 +3790,22 @@
         <v>0.00252</v>
       </c>
       <c r="Q3" s="6" t="n">
-        <v>0.01755</v>
+        <v>0.01773</v>
       </c>
       <c r="R3" s="6" t="n">
-        <v>0.0099</v>
+        <v>0.00999</v>
       </c>
       <c r="S3" s="6" t="n">
-        <v>0.00747</v>
+        <v>0.00756</v>
       </c>
       <c r="T3" s="6" t="n">
-        <v>0.01242</v>
+        <v>0.01251</v>
       </c>
       <c r="U3" s="6" t="n">
-        <v>0.02979</v>
+        <v>0.02997</v>
       </c>
       <c r="V3" s="6" t="n">
-        <v>0.12168</v>
+        <v>0.12276</v>
       </c>
     </row>
     <row r="4">
@@ -3846,7 +3846,7 @@
         <v>0.0063</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>0.0252</v>
+        <v>0.0189</v>
       </c>
       <c r="N4" s="6" t="n">
         <v>0.0063</v>
@@ -3858,7 +3858,7 @@
         <v>0.0063</v>
       </c>
       <c r="Q4" s="6" t="n">
-        <v>0.0252</v>
+        <v>0.0189</v>
       </c>
       <c r="R4" s="6" t="n">
         <v>0.0063</v>
@@ -3870,7 +3870,7 @@
         <v>0.0063</v>
       </c>
       <c r="U4" s="6" t="n">
-        <v>0.0252</v>
+        <v>0.0189</v>
       </c>
       <c r="V4" s="6" t="n">
         <v>0.0756</v>
@@ -4224,7 +4224,7 @@
         <v>0.0118</v>
       </c>
       <c r="U2" s="7" t="n">
-        <v>0.0273</v>
+        <v>0.0274</v>
       </c>
       <c r="V2" s="7" t="n">
         <v>0.0804</v>
@@ -4292,7 +4292,7 @@
         <v>0.01062</v>
       </c>
       <c r="U3" s="7" t="n">
-        <v>0.02457</v>
+        <v>0.02466</v>
       </c>
       <c r="V3" s="7" t="n">
         <v>0.07236</v>
@@ -4336,7 +4336,7 @@
         <v>0.0094</v>
       </c>
       <c r="M4" s="7" t="n">
-        <v>0.0376</v>
+        <v>0.0282</v>
       </c>
       <c r="N4" s="7" t="n">
         <v>0.0094</v>
@@ -4348,7 +4348,7 @@
         <v>0.0094</v>
       </c>
       <c r="Q4" s="7" t="n">
-        <v>0.0376</v>
+        <v>0.0282</v>
       </c>
       <c r="R4" s="7" t="n">
         <v>0.0094</v>
@@ -4360,7 +4360,7 @@
         <v>0.0094</v>
       </c>
       <c r="U4" s="7" t="n">
-        <v>0.0376</v>
+        <v>0.0282</v>
       </c>
       <c r="V4" s="7" t="n">
         <v>0.1128</v>
@@ -4667,55 +4667,55 @@
         <v>25</v>
       </c>
       <c r="F2" s="8" t="n">
-        <v>0.0063</v>
+        <v>0.008</v>
       </c>
       <c r="G2" s="8" t="n">
-        <v>0.0062</v>
+        <v>0.0078</v>
       </c>
       <c r="H2" s="8" t="n">
-        <v>0.0061</v>
+        <v>0.0078</v>
       </c>
       <c r="I2" s="8" t="n">
-        <v>0.0186</v>
+        <v>0.0236</v>
       </c>
       <c r="J2" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K2" s="8" t="n">
-        <v>0.012</v>
+        <v>0.015</v>
       </c>
       <c r="L2" s="8" t="n">
-        <v>0.0118</v>
+        <v>0.0148</v>
       </c>
       <c r="M2" s="8" t="n">
-        <v>0.0239</v>
+        <v>0.03</v>
       </c>
       <c r="N2" s="8" t="n">
-        <v>0.0059</v>
+        <v>0.0074</v>
       </c>
       <c r="O2" s="8" t="n">
-        <v>0.0059</v>
+        <v>0.0074</v>
       </c>
       <c r="P2" s="8" t="n">
-        <v>0.018</v>
+        <v>0.0226</v>
       </c>
       <c r="Q2" s="8" t="n">
-        <v>0.0297</v>
+        <v>0.0372</v>
       </c>
       <c r="R2" s="8" t="n">
         <v>0</v>
       </c>
       <c r="S2" s="8" t="n">
-        <v>0.0118</v>
+        <v>0.0147</v>
       </c>
       <c r="T2" s="8" t="n">
-        <v>0.0118</v>
+        <v>0.0147</v>
       </c>
       <c r="U2" s="8" t="n">
-        <v>0.0236</v>
+        <v>0.0295</v>
       </c>
       <c r="V2" s="8" t="n">
-        <v>0.096</v>
+        <v>0.1206</v>
       </c>
     </row>
     <row r="3">
@@ -4735,55 +4735,55 @@
         <v>26</v>
       </c>
       <c r="F3" s="8" t="n">
-        <v>0.00567</v>
+        <v>0.0072</v>
       </c>
       <c r="G3" s="8" t="n">
-        <v>0.00558</v>
+        <v>0.00702</v>
       </c>
       <c r="H3" s="8" t="n">
-        <v>0.00549</v>
+        <v>0.00702</v>
       </c>
       <c r="I3" s="8" t="n">
-        <v>0.01674</v>
+        <v>0.02124</v>
       </c>
       <c r="J3" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="8" t="n">
-        <v>0.0108</v>
+        <v>0.0135</v>
       </c>
       <c r="L3" s="8" t="n">
-        <v>0.01062</v>
+        <v>0.01332</v>
       </c>
       <c r="M3" s="8" t="n">
-        <v>0.02151</v>
+        <v>0.027</v>
       </c>
       <c r="N3" s="8" t="n">
-        <v>0.00531</v>
+        <v>0.00666</v>
       </c>
       <c r="O3" s="8" t="n">
-        <v>0.00531</v>
+        <v>0.00666</v>
       </c>
       <c r="P3" s="8" t="n">
-        <v>0.0162</v>
+        <v>0.02034</v>
       </c>
       <c r="Q3" s="8" t="n">
-        <v>0.02673</v>
+        <v>0.03348</v>
       </c>
       <c r="R3" s="8" t="n">
         <v>0</v>
       </c>
       <c r="S3" s="8" t="n">
-        <v>0.01062</v>
+        <v>0.01323</v>
       </c>
       <c r="T3" s="8" t="n">
-        <v>0.01062</v>
+        <v>0.01323</v>
       </c>
       <c r="U3" s="8" t="n">
-        <v>0.02124</v>
+        <v>0.02655</v>
       </c>
       <c r="V3" s="8" t="n">
-        <v>0.0864</v>
+        <v>0.10854</v>
       </c>
     </row>
     <row r="4">
@@ -4824,7 +4824,7 @@
         <v>0.0073</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>0.0292</v>
+        <v>0.0219</v>
       </c>
       <c r="N4" s="8" t="n">
         <v>0.0073</v>
@@ -4836,7 +4836,7 @@
         <v>0.0073</v>
       </c>
       <c r="Q4" s="8" t="n">
-        <v>0.0292</v>
+        <v>0.0219</v>
       </c>
       <c r="R4" s="8" t="n">
         <v>0.0073</v>
@@ -4848,7 +4848,7 @@
         <v>0.0073</v>
       </c>
       <c r="U4" s="8" t="n">
-        <v>0.0292</v>
+        <v>0.0219</v>
       </c>
       <c r="V4" s="8" t="n">
         <v>0.0876</v>
@@ -5304,7 +5304,7 @@
         <v>0.01515</v>
       </c>
       <c r="M4" s="9" t="n">
-        <v>0.0606</v>
+        <v>0.04545</v>
       </c>
       <c r="N4" s="9" t="n">
         <v>0.01515</v>
@@ -5316,7 +5316,7 @@
         <v>0.01515</v>
       </c>
       <c r="Q4" s="9" t="n">
-        <v>0.0606</v>
+        <v>0.04545</v>
       </c>
       <c r="R4" s="9" t="n">
         <v>0.01515</v>
@@ -5328,7 +5328,7 @@
         <v>0.01515</v>
       </c>
       <c r="U4" s="9" t="n">
-        <v>0.0606</v>
+        <v>0.04545</v>
       </c>
       <c r="V4" s="9" t="n">
         <v>0.1818</v>

</xml_diff>

<commit_message>
Didn't previously update automate_finance.qmd to use the updated CVD files, need to make that dynamic.
</commit_message>
<xml_diff>
--- a/outputs/BURs/BUR Testing_AMC.xlsx
+++ b/outputs/BURs/BUR Testing_AMC.xlsx
@@ -577,7 +577,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -645,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -713,7 +713,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -728,46 +728,46 @@
         <v>0.0192</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.0383</v>
+        <v>0.0381</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>0.0115</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0038</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0106583333333333</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.03735</v>
+        <v>0.031975</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0106583333333333</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0106583333333333</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0106583333333333</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>0.03735</v>
+        <v>0.031975</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0106583333333333</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0106583333333333</v>
       </c>
       <c r="T4" s="1" t="n">
-        <v>0.01245</v>
+        <v>0.0106583333333333</v>
       </c>
       <c r="U4" s="1" t="n">
-        <v>0.03735</v>
+        <v>0.031975</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>0.1494</v>
+        <v>0.1279</v>
       </c>
     </row>
     <row r="5">
@@ -781,7 +781,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -849,7 +849,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -917,61 +917,61 @@
         <v>28</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="1" t="n">
+        <v>0.1429</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="G7" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>0.3077</v>
-      </c>
       <c r="J7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.4286</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="O7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="R7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="T7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="U7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="V7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.285714285714286</v>
       </c>
     </row>
   </sheetData>
@@ -1067,7 +1067,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="10" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -1135,7 +1135,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="10" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -1203,7 +1203,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -1212,52 +1212,52 @@
         <v>0</v>
       </c>
       <c r="G4" s="10" t="n">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="10" t="n">
-        <v>0.8511</v>
+        <v>1.0811</v>
       </c>
       <c r="J4" s="10" t="n">
         <v>0</v>
       </c>
       <c r="K4" s="10" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="L4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="M4" s="10" t="n">
-        <v>0.75</v>
+        <v>0.9231</v>
       </c>
       <c r="N4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="O4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="P4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="Q4" s="10" t="n">
-        <v>0.75</v>
+        <v>0.9231</v>
       </c>
       <c r="R4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="S4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="T4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="U4" s="10" t="n">
-        <v>0.75</v>
+        <v>0.9231</v>
       </c>
       <c r="V4" s="10" t="n">
-        <v>3</v>
+        <v>3.6924</v>
       </c>
     </row>
     <row r="5">
@@ -1473,7 +1473,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="11" t="n">
-        <v>0.0366</v>
+        <v>0.0454</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -1541,7 +1541,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="11" t="n">
-        <v>0.0366</v>
+        <v>0.0454</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -1609,7 +1609,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="11" t="n">
-        <v>0.0366</v>
+        <v>0.0454</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -1630,40 +1630,40 @@
         <v>0.01</v>
       </c>
       <c r="K4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.0089</v>
       </c>
       <c r="L4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.00908333333333333</v>
       </c>
       <c r="M4" s="11" t="n">
-        <v>0.02745</v>
+        <v>0.02725</v>
       </c>
       <c r="N4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.00908333333333333</v>
       </c>
       <c r="O4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.00908333333333333</v>
       </c>
       <c r="P4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.00908333333333333</v>
       </c>
       <c r="Q4" s="11" t="n">
-        <v>0.02745</v>
+        <v>0.02725</v>
       </c>
       <c r="R4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.00908333333333333</v>
       </c>
       <c r="S4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.00908333333333333</v>
       </c>
       <c r="T4" s="11" t="n">
-        <v>0.00915</v>
+        <v>0.00908333333333333</v>
       </c>
       <c r="U4" s="11" t="n">
-        <v>0.02745</v>
+        <v>0.02725</v>
       </c>
       <c r="V4" s="11" t="n">
-        <v>0.1098</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="5">
@@ -1677,7 +1677,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1745,7 +1745,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -1813,16 +1813,16 @@
         <v>28</v>
       </c>
       <c r="D7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="11" t="n">
-        <v>0.5357</v>
+        <v>0.5185</v>
       </c>
       <c r="G7" s="11" t="n">
-        <v>0.6296</v>
+        <v>0.6429</v>
       </c>
       <c r="H7" s="11" t="n">
         <v>0.8</v>
@@ -1831,43 +1831,43 @@
         <v>0.6286</v>
       </c>
       <c r="J7" s="11" t="n">
-        <v>0.65</v>
+        <v>0.7</v>
       </c>
       <c r="K7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.6364</v>
       </c>
       <c r="L7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="M7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="N7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="O7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="P7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="Q7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="R7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="S7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="T7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="U7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
       <c r="V7" s="11" t="n">
-        <v>0.633333333333333</v>
+        <v>0.642857142857143</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +1963,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2031,7 +2031,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2099,7 +2099,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -2117,43 +2117,43 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0</v>
+        <v>0.0083</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0</v>
+        <v>0.00165833333333333</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0</v>
+        <v>0.004975</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0</v>
+        <v>0.00165833333333333</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>0</v>
+        <v>0.00165833333333333</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>0</v>
+        <v>0.00165833333333333</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>0</v>
+        <v>0.004975</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>0</v>
+        <v>0.00165833333333333</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>0</v>
+        <v>0.00165833333333333</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>0</v>
+        <v>0.00165833333333333</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>0</v>
+        <v>0.004975</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>0</v>
+        <v>0.0199</v>
       </c>
     </row>
     <row r="5">
@@ -2167,7 +2167,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
@@ -2184,40 +2184,40 @@
         <v>1</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="T5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="U5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -2313,7 +2313,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2381,7 +2381,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2449,7 +2449,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -2458,10 +2458,10 @@
         <v>0.0088</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>0.007</v>
+        <v>0.0071</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>0.016</v>
+        <v>0.0161</v>
       </c>
       <c r="I4" s="3" t="n">
         <v>0.0319</v>
@@ -2470,40 +2470,40 @@
         <v>0.0126</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0072</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0103583333333333</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0.0333</v>
+        <v>0.031075</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0103583333333333</v>
       </c>
       <c r="O4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0103583333333333</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0103583333333333</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>0.0333</v>
+        <v>0.031075</v>
       </c>
       <c r="R4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0103583333333333</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0103583333333333</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>0.0111</v>
+        <v>0.0103583333333333</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>0.0333</v>
+        <v>0.031075</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>0.1332</v>
+        <v>0.1243</v>
       </c>
     </row>
     <row r="5">
@@ -2517,7 +2517,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -2585,7 +2585,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -2653,7 +2653,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -2674,40 +2674,40 @@
         <v>0.8</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.7143</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="P7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="R7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="S7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="T7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="U7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
       <c r="V7" s="3" t="n">
-        <v>0.55</v>
+        <v>0.592592592592593</v>
       </c>
     </row>
   </sheetData>
@@ -2803,7 +2803,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2871,7 +2871,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2939,7 +2939,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -3193,7 +3193,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3261,7 +3261,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -3329,7 +3329,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -3341,49 +3341,49 @@
         <v>0.0061</v>
       </c>
       <c r="H4" s="5" t="n">
+        <v>0.0061</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0.0223</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>0.0082</v>
+      </c>
+      <c r="K4" s="5" t="n">
         <v>0.0062</v>
       </c>
-      <c r="I4" s="5" t="n">
-        <v>0.0225</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>0.0083</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>0.007675</v>
-      </c>
       <c r="L4" s="5" t="n">
-        <v>0.007675</v>
+        <v>0.00735833333333333</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>0.023025</v>
+        <v>0.022075</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>0.007675</v>
+        <v>0.00735833333333333</v>
       </c>
       <c r="O4" s="5" t="n">
-        <v>0.007675</v>
+        <v>0.00735833333333333</v>
       </c>
       <c r="P4" s="5" t="n">
-        <v>0.007675</v>
+        <v>0.00735833333333333</v>
       </c>
       <c r="Q4" s="5" t="n">
-        <v>0.023025</v>
+        <v>0.022075</v>
       </c>
       <c r="R4" s="5" t="n">
-        <v>0.007675</v>
+        <v>0.00735833333333333</v>
       </c>
       <c r="S4" s="5" t="n">
-        <v>0.007675</v>
+        <v>0.00735833333333333</v>
       </c>
       <c r="T4" s="5" t="n">
-        <v>0.007675</v>
+        <v>0.00735833333333333</v>
       </c>
       <c r="U4" s="5" t="n">
-        <v>0.023025</v>
+        <v>0.022075</v>
       </c>
       <c r="V4" s="5" t="n">
-        <v>0.0921</v>
+        <v>0.0883</v>
       </c>
     </row>
     <row r="5">
@@ -3397,7 +3397,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -3465,7 +3465,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -3533,7 +3533,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -3551,43 +3551,43 @@
         <v>0.8333</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>0.3333</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="O7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="P7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="Q7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="R7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="S7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="T7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="U7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="V7" s="5" t="n">
-        <v>0.733333333333333</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>
@@ -3683,7 +3683,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3751,7 +3751,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -3819,7 +3819,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -3834,46 +3834,46 @@
         <v>0.0084</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>0.0139</v>
+        <v>0.014</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>0.0114</v>
+        <v>0.0085</v>
       </c>
       <c r="K4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.0058</v>
       </c>
       <c r="L4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.00564166666666667</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>0.0189</v>
+        <v>0.016925</v>
       </c>
       <c r="N4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.00564166666666667</v>
       </c>
       <c r="O4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.00564166666666667</v>
       </c>
       <c r="P4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.00564166666666667</v>
       </c>
       <c r="Q4" s="6" t="n">
-        <v>0.0189</v>
+        <v>0.016925</v>
       </c>
       <c r="R4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.00564166666666667</v>
       </c>
       <c r="S4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.00564166666666667</v>
       </c>
       <c r="T4" s="6" t="n">
-        <v>0.0063</v>
+        <v>0.00564166666666667</v>
       </c>
       <c r="U4" s="6" t="n">
-        <v>0.0189</v>
+        <v>0.016925</v>
       </c>
       <c r="V4" s="6" t="n">
-        <v>0.0756</v>
+        <v>0.0677</v>
       </c>
     </row>
     <row r="5">
@@ -4043,9 +4043,7 @@
       <c r="J7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="6" t="n">
-        <v>0.888888888888889</v>
-      </c>
+      <c r="K7" s="6"/>
       <c r="L7" s="6" t="n">
         <v>0.888888888888889</v>
       </c>
@@ -4173,7 +4171,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -4241,7 +4239,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -4309,61 +4307,61 @@
         <v>24</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>0.0139</v>
+        <v>0.0138</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>0.0079</v>
+        <v>0.0078</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0.0063</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>0.0282</v>
+        <v>0.028</v>
       </c>
       <c r="J4" s="7" t="n">
         <v>0.0094</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0158</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0106166666666667</v>
       </c>
       <c r="M4" s="7" t="n">
-        <v>0.0282</v>
+        <v>0.03185</v>
       </c>
       <c r="N4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0106166666666667</v>
       </c>
       <c r="O4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0106166666666667</v>
       </c>
       <c r="P4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0106166666666667</v>
       </c>
       <c r="Q4" s="7" t="n">
-        <v>0.0282</v>
+        <v>0.03185</v>
       </c>
       <c r="R4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0106166666666667</v>
       </c>
       <c r="S4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0106166666666667</v>
       </c>
       <c r="T4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0106166666666667</v>
       </c>
       <c r="U4" s="7" t="n">
-        <v>0.0282</v>
+        <v>0.03185</v>
       </c>
       <c r="V4" s="7" t="n">
-        <v>0.1128</v>
+        <v>0.1274</v>
       </c>
     </row>
     <row r="5">
@@ -4377,7 +4375,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -4443,7 +4441,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -4511,7 +4509,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -4532,40 +4530,40 @@
         <v>0.8</v>
       </c>
       <c r="K7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>1</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="M7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="O7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="P7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="Q7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="R7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="S7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="T7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="U7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="V7" s="7" t="n">
-        <v>0.842105263157895</v>
+        <v>0.857142857142857</v>
       </c>
     </row>
   </sheetData>
@@ -4661,7 +4659,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="8" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -4729,7 +4727,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="8" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -4797,7 +4795,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="8" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -4818,40 +4816,40 @@
         <v>0.0116</v>
       </c>
       <c r="K4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.0179</v>
       </c>
       <c r="L4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.00938333333333333</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>0.0219</v>
+        <v>0.02815</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.00938333333333333</v>
       </c>
       <c r="O4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.00938333333333333</v>
       </c>
       <c r="P4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.00938333333333333</v>
       </c>
       <c r="Q4" s="8" t="n">
-        <v>0.0219</v>
+        <v>0.02815</v>
       </c>
       <c r="R4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.00938333333333333</v>
       </c>
       <c r="S4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.00938333333333333</v>
       </c>
       <c r="T4" s="8" t="n">
-        <v>0.0073</v>
+        <v>0.00938333333333333</v>
       </c>
       <c r="U4" s="8" t="n">
-        <v>0.0219</v>
+        <v>0.02815</v>
       </c>
       <c r="V4" s="8" t="n">
-        <v>0.0876</v>
+        <v>0.1126</v>
       </c>
     </row>
     <row r="5">
@@ -4865,7 +4863,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -4923,7 +4921,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -4991,7 +4989,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -5000,52 +4998,52 @@
         <v>0</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="8" t="n">
         <v>1</v>
       </c>
       <c r="I7" s="8" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="J7" s="8" t="n">
         <v>1</v>
       </c>
       <c r="K7" s="8" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="L7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="M7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="N7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="O7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="P7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="Q7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="R7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="S7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="T7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="U7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="V7" s="8" t="n">
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
     </row>
   </sheetData>
@@ -5141,7 +5139,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="9" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -5209,7 +5207,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -5277,7 +5275,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="9" t="n">
-        <v>0.0498</v>
+        <v>0.0533</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -5298,40 +5296,40 @@
         <v>0</v>
       </c>
       <c r="K4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0</v>
       </c>
       <c r="L4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0.0120416666666667</v>
       </c>
       <c r="M4" s="9" t="n">
-        <v>0.04545</v>
+        <v>0.036125</v>
       </c>
       <c r="N4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0.0120416666666667</v>
       </c>
       <c r="O4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0.0120416666666667</v>
       </c>
       <c r="P4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0.0120416666666667</v>
       </c>
       <c r="Q4" s="9" t="n">
-        <v>0.04545</v>
+        <v>0.036125</v>
       </c>
       <c r="R4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0.0120416666666667</v>
       </c>
       <c r="S4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0.0120416666666667</v>
       </c>
       <c r="T4" s="9" t="n">
-        <v>0.01515</v>
+        <v>0.0120416666666667</v>
       </c>
       <c r="U4" s="9" t="n">
-        <v>0.04545</v>
+        <v>0.036125</v>
       </c>
       <c r="V4" s="9" t="n">
-        <v>0.1818</v>
+        <v>0.1445</v>
       </c>
     </row>
     <row r="5">
@@ -5485,9 +5483,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="9"/>
-      <c r="K7" s="9" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="K7" s="9"/>
       <c r="L7" s="9" t="n">
         <v>0.5</v>
       </c>

</xml_diff>

<commit_message>
Updated IPS AIP hipo turnover
</commit_message>
<xml_diff>
--- a/outputs/BURs/BUR Testing_AMC.xlsx
+++ b/outputs/BURs/BUR Testing_AMC.xlsx
@@ -577,7 +577,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.0533</v>
+        <v>0.0606</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -645,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.0533</v>
+        <v>0.0606</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -713,7 +713,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.0533</v>
+        <v>0.0606</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -737,37 +737,37 @@
         <v>0.0038</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.0106583333333333</v>
+        <v>0.0074</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.031975</v>
+        <v>0.0226</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>0.0106583333333333</v>
+        <v>0.0101</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>0.0106583333333333</v>
+        <v>0.0101</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>0.0106583333333333</v>
+        <v>0.0101</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>0.031975</v>
+        <v>0.0303</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.0106583333333333</v>
+        <v>0.0101</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0.0106583333333333</v>
+        <v>0.0101</v>
       </c>
       <c r="T4" s="1" t="n">
-        <v>0.0106583333333333</v>
+        <v>0.0101</v>
       </c>
       <c r="U4" s="1" t="n">
-        <v>0.031975</v>
+        <v>0.0303</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>0.1279</v>
+        <v>0.1212</v>
       </c>
     </row>
     <row r="5">
@@ -781,7 +781,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -849,7 +849,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -917,13 +917,13 @@
         <v>28</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>0.1429</v>
+        <v>0.25</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>0.5</v>
@@ -932,46 +932,46 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>0.25</v>
+        <v>0.3077</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>0.4286</v>
+        <v>0.3333</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.2</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.2308</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="O7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="R7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="T7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="U7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
       <c r="V7" s="1" t="n">
-        <v>0.285714285714286</v>
+        <v>0.269230769230769</v>
       </c>
     </row>
   </sheetData>
@@ -1067,7 +1067,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="10" t="n">
-        <v>0.0533</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -1135,7 +1135,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="10" t="n">
-        <v>0.0533</v>
+        <v>0.5</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -1203,7 +1203,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>0.0533</v>
+        <v>0.5</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -1212,52 +1212,42 @@
         <v>0</v>
       </c>
       <c r="G4" s="10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="10" t="n">
-        <v>2</v>
-      </c>
+        <v>0.6667</v>
+      </c>
+      <c r="H4" s="10"/>
       <c r="I4" s="10" t="n">
-        <v>1.0811</v>
-      </c>
-      <c r="J4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10" t="n">
-        <v>0.3077</v>
-      </c>
-      <c r="M4" s="10" t="n">
-        <v>0.9231</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
       <c r="N4" s="10" t="n">
-        <v>0.3077</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="O4" s="10" t="n">
-        <v>0.3077</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="P4" s="10" t="n">
-        <v>0.3077</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="Q4" s="10" t="n">
-        <v>0.9231</v>
+        <v>0.25</v>
       </c>
       <c r="R4" s="10" t="n">
-        <v>0.3077</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="S4" s="10" t="n">
-        <v>0.3077</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="T4" s="10" t="n">
-        <v>0.3077</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="U4" s="10" t="n">
-        <v>0.9231</v>
+        <v>0.25</v>
       </c>
       <c r="V4" s="10" t="n">
-        <v>3.6924</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1473,7 +1463,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="11" t="n">
-        <v>0.0454</v>
+        <v>0.0522</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -1541,7 +1531,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="11" t="n">
-        <v>0.0454</v>
+        <v>0.0522</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -1609,13 +1599,13 @@
         <v>24</v>
       </c>
       <c r="D4" s="11" t="n">
-        <v>0.0454</v>
+        <v>0.0522</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="11" t="n">
-        <v>0.0087</v>
+        <v>0.0086</v>
       </c>
       <c r="G4" s="11" t="n">
         <v>0.0076</v>
@@ -1624,46 +1614,46 @@
         <v>0.0103</v>
       </c>
       <c r="I4" s="11" t="n">
-        <v>0.0266</v>
+        <v>0.0265</v>
       </c>
       <c r="J4" s="11" t="n">
-        <v>0.01</v>
+        <v>0.0099</v>
       </c>
       <c r="K4" s="11" t="n">
-        <v>0.0089</v>
+        <v>0.0085</v>
       </c>
       <c r="L4" s="11" t="n">
-        <v>0.00908333333333333</v>
+        <v>0.0073</v>
       </c>
       <c r="M4" s="11" t="n">
-        <v>0.02725</v>
+        <v>0.0257</v>
       </c>
       <c r="N4" s="11" t="n">
-        <v>0.00908333333333333</v>
+        <v>0.0087</v>
       </c>
       <c r="O4" s="11" t="n">
-        <v>0.00908333333333333</v>
+        <v>0.0087</v>
       </c>
       <c r="P4" s="11" t="n">
-        <v>0.00908333333333333</v>
+        <v>0.0087</v>
       </c>
       <c r="Q4" s="11" t="n">
-        <v>0.02725</v>
+        <v>0.0261</v>
       </c>
       <c r="R4" s="11" t="n">
-        <v>0.00908333333333333</v>
+        <v>0.0087</v>
       </c>
       <c r="S4" s="11" t="n">
-        <v>0.00908333333333333</v>
+        <v>0.0087</v>
       </c>
       <c r="T4" s="11" t="n">
-        <v>0.00908333333333333</v>
+        <v>0.0087</v>
       </c>
       <c r="U4" s="11" t="n">
-        <v>0.02725</v>
+        <v>0.0261</v>
       </c>
       <c r="V4" s="11" t="n">
-        <v>0.109</v>
+        <v>0.1044</v>
       </c>
     </row>
     <row r="5">
@@ -1677,7 +1667,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1745,7 +1735,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -1813,13 +1803,13 @@
         <v>28</v>
       </c>
       <c r="D7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="11" t="n">
-        <v>0.5185</v>
+        <v>0.5357</v>
       </c>
       <c r="G7" s="11" t="n">
         <v>0.6429</v>
@@ -1828,7 +1818,7 @@
         <v>0.8</v>
       </c>
       <c r="I7" s="11" t="n">
-        <v>0.6286</v>
+        <v>0.6338</v>
       </c>
       <c r="J7" s="11" t="n">
         <v>0.7</v>
@@ -1837,37 +1827,37 @@
         <v>0.6364</v>
       </c>
       <c r="L7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.5385</v>
       </c>
       <c r="M7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.6364</v>
       </c>
       <c r="N7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="O7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="P7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="Q7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="R7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="S7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="T7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="U7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
       <c r="V7" s="11" t="n">
-        <v>0.642857142857143</v>
+        <v>0.634920634920635</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +1953,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.0533</v>
+        <v>0.0081</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2031,7 +2021,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.0533</v>
+        <v>0.0081</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2099,7 +2089,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.0533</v>
+        <v>0.0081</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -2123,37 +2113,37 @@
         <v>0</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.00165833333333333</v>
+        <v>0</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0.004975</v>
+        <v>0.008</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0.00165833333333333</v>
+        <v>0.00135</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>0.00165833333333333</v>
+        <v>0.00135</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>0.00165833333333333</v>
+        <v>0.00135</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>0.004975</v>
+        <v>0.00405</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>0.00165833333333333</v>
+        <v>0.00135</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>0.00165833333333333</v>
+        <v>0.00135</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>0.00165833333333333</v>
+        <v>0.00135</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>0.004975</v>
+        <v>0.00405</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>0.0199</v>
+        <v>0.0162</v>
       </c>
     </row>
     <row r="5">
@@ -2186,11 +2176,9 @@
       <c r="K5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="L5" s="2" t="n">
-        <v>0.666666666666667</v>
-      </c>
+      <c r="L5" s="2"/>
       <c r="M5" s="2" t="n">
-        <v>0.666666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0.666666666666667</v>
@@ -2313,7 +2301,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.0533</v>
+        <v>0.0619</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2381,7 +2369,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.0533</v>
+        <v>0.0619</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2449,61 +2437,61 @@
         <v>24</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.0533</v>
+        <v>0.0619</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0.0088</v>
+        <v>0.0087</v>
       </c>
       <c r="G4" s="3" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0.0159</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <v>0.0315</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="K4" s="3" t="n">
         <v>0.0071</v>
       </c>
-      <c r="H4" s="3" t="n">
-        <v>0.0161</v>
-      </c>
-      <c r="I4" s="3" t="n">
-        <v>0.0319</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>0.0126</v>
-      </c>
-      <c r="K4" s="3" t="n">
-        <v>0.0072</v>
-      </c>
       <c r="L4" s="3" t="n">
-        <v>0.0103583333333333</v>
+        <v>0.0108</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0.031075</v>
+        <v>0.0304</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>0.0103583333333333</v>
+        <v>0.0103166666666667</v>
       </c>
       <c r="O4" s="3" t="n">
-        <v>0.0103583333333333</v>
+        <v>0.0103166666666667</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>0.0103583333333333</v>
+        <v>0.0103166666666667</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>0.031075</v>
+        <v>0.03095</v>
       </c>
       <c r="R4" s="3" t="n">
-        <v>0.0103583333333333</v>
+        <v>0.0103166666666667</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>0.0103583333333333</v>
+        <v>0.0103166666666667</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>0.0103583333333333</v>
+        <v>0.0103166666666667</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>0.031075</v>
+        <v>0.03095</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>0.1243</v>
+        <v>0.1238</v>
       </c>
     </row>
     <row r="5">
@@ -2517,7 +2505,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -2585,7 +2573,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -2653,7 +2641,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -2677,37 +2665,37 @@
         <v>0.7143</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6667</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.7333</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="P7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="R7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="S7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="T7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="U7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
       <c r="V7" s="3" t="n">
-        <v>0.592592592592593</v>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -2803,7 +2791,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>0.0533</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2871,7 +2859,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>0.0533</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2939,7 +2927,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.0533</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -3193,7 +3181,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.0533</v>
+        <v>0.0367</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3261,7 +3249,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.0533</v>
+        <v>0.0367</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -3329,7 +3317,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.0533</v>
+        <v>0.0367</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -3350,40 +3338,40 @@
         <v>0.0082</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>0.0062</v>
+        <v>0.0041</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>0.00735833333333333</v>
+        <v>0.002</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>0.022075</v>
+        <v>0.0144</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>0.00735833333333333</v>
+        <v>0.00611666666666667</v>
       </c>
       <c r="O4" s="5" t="n">
-        <v>0.00735833333333333</v>
+        <v>0.00611666666666667</v>
       </c>
       <c r="P4" s="5" t="n">
-        <v>0.00735833333333333</v>
+        <v>0.00611666666666667</v>
       </c>
       <c r="Q4" s="5" t="n">
-        <v>0.022075</v>
+        <v>0.01835</v>
       </c>
       <c r="R4" s="5" t="n">
-        <v>0.00735833333333333</v>
+        <v>0.00611666666666667</v>
       </c>
       <c r="S4" s="5" t="n">
-        <v>0.00735833333333333</v>
+        <v>0.00611666666666667</v>
       </c>
       <c r="T4" s="5" t="n">
-        <v>0.00735833333333333</v>
+        <v>0.00611666666666667</v>
       </c>
       <c r="U4" s="5" t="n">
-        <v>0.022075</v>
+        <v>0.01835</v>
       </c>
       <c r="V4" s="5" t="n">
-        <v>0.0883</v>
+        <v>0.0734</v>
       </c>
     </row>
     <row r="5">
@@ -3397,7 +3385,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -3465,7 +3453,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -3533,7 +3521,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -3557,37 +3545,37 @@
         <v>0.75</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.6667</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="O7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="P7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="Q7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="R7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="S7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="T7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="U7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="V7" s="5" t="n">
-        <v>0.75</v>
+        <v>0.761904761904762</v>
       </c>
     </row>
   </sheetData>
@@ -3683,7 +3671,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>0.0533</v>
+        <v>0.031</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3751,7 +3739,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>0.0533</v>
+        <v>0.031</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -3819,7 +3807,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>0.0533</v>
+        <v>0.031</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -3834,46 +3822,46 @@
         <v>0.0084</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>0.014</v>
+        <v>0.0139</v>
       </c>
       <c r="J4" s="6" t="n">
         <v>0.0085</v>
       </c>
       <c r="K4" s="6" t="n">
-        <v>0.0058</v>
+        <v>0.0057</v>
       </c>
       <c r="L4" s="6" t="n">
-        <v>0.00564166666666667</v>
+        <v>0.0029</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>0.016925</v>
+        <v>0.0171</v>
       </c>
       <c r="N4" s="6" t="n">
-        <v>0.00564166666666667</v>
+        <v>0.00516666666666667</v>
       </c>
       <c r="O4" s="6" t="n">
-        <v>0.00564166666666667</v>
+        <v>0.00516666666666667</v>
       </c>
       <c r="P4" s="6" t="n">
-        <v>0.00564166666666667</v>
+        <v>0.00516666666666667</v>
       </c>
       <c r="Q4" s="6" t="n">
-        <v>0.016925</v>
+        <v>0.0155</v>
       </c>
       <c r="R4" s="6" t="n">
-        <v>0.00564166666666667</v>
+        <v>0.00516666666666667</v>
       </c>
       <c r="S4" s="6" t="n">
-        <v>0.00564166666666667</v>
+        <v>0.00516666666666667</v>
       </c>
       <c r="T4" s="6" t="n">
-        <v>0.00564166666666667</v>
+        <v>0.00516666666666667</v>
       </c>
       <c r="U4" s="6" t="n">
-        <v>0.016925</v>
+        <v>0.0155</v>
       </c>
       <c r="V4" s="6" t="n">
-        <v>0.0677</v>
+        <v>0.062</v>
       </c>
     </row>
     <row r="5">
@@ -4044,11 +4032,9 @@
         <v>1</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="6" t="n">
-        <v>0.888888888888889</v>
-      </c>
+      <c r="L7" s="6"/>
       <c r="M7" s="6" t="n">
-        <v>0.888888888888889</v>
+        <v>1</v>
       </c>
       <c r="N7" s="6" t="n">
         <v>0.888888888888889</v>
@@ -4171,7 +4157,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>0.0533</v>
+        <v>0.0647</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -4239,7 +4225,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>0.0533</v>
+        <v>0.0647</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -4307,61 +4293,61 @@
         <v>24</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>0.0533</v>
+        <v>0.0647</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>0.0138</v>
+        <v>0.0139</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>0.0078</v>
+        <v>0.0079</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0.0063</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>0.028</v>
+        <v>0.0282</v>
       </c>
       <c r="J4" s="7" t="n">
         <v>0.0094</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>0.0158</v>
+        <v>0.0159</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>0.0106166666666667</v>
+        <v>0.0112</v>
       </c>
       <c r="M4" s="7" t="n">
-        <v>0.03185</v>
+        <v>0.0365</v>
       </c>
       <c r="N4" s="7" t="n">
-        <v>0.0106166666666667</v>
+        <v>0.0107833333333333</v>
       </c>
       <c r="O4" s="7" t="n">
-        <v>0.0106166666666667</v>
+        <v>0.0107833333333333</v>
       </c>
       <c r="P4" s="7" t="n">
-        <v>0.0106166666666667</v>
+        <v>0.0107833333333333</v>
       </c>
       <c r="Q4" s="7" t="n">
-        <v>0.03185</v>
+        <v>0.03235</v>
       </c>
       <c r="R4" s="7" t="n">
-        <v>0.0106166666666667</v>
+        <v>0.0107833333333333</v>
       </c>
       <c r="S4" s="7" t="n">
-        <v>0.0106166666666667</v>
+        <v>0.0107833333333333</v>
       </c>
       <c r="T4" s="7" t="n">
-        <v>0.0106166666666667</v>
+        <v>0.0107833333333333</v>
       </c>
       <c r="U4" s="7" t="n">
-        <v>0.03185</v>
+        <v>0.03235</v>
       </c>
       <c r="V4" s="7" t="n">
-        <v>0.1274</v>
+        <v>0.1294</v>
       </c>
     </row>
     <row r="5">
@@ -4375,7 +4361,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -4441,7 +4427,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -4509,7 +4495,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -4533,37 +4519,37 @@
         <v>1</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.75</v>
       </c>
       <c r="M7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.8333</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="O7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="P7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="Q7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="R7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="S7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="T7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="U7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
       <c r="V7" s="7" t="n">
-        <v>0.857142857142857</v>
+        <v>0.846153846153846</v>
       </c>
     </row>
   </sheetData>
@@ -4659,7 +4645,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="8" t="n">
-        <v>0.0533</v>
+        <v>0.0526</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -4727,7 +4713,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="8" t="n">
-        <v>0.0533</v>
+        <v>0.0526</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -4795,7 +4781,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="8" t="n">
-        <v>0.0533</v>
+        <v>0.0526</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -4804,52 +4790,52 @@
         <v>0.0058</v>
       </c>
       <c r="G4" s="8" t="n">
-        <v>0.0117</v>
+        <v>0.0116</v>
       </c>
       <c r="H4" s="8" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>0.0176</v>
+        <v>0.0175</v>
       </c>
       <c r="J4" s="8" t="n">
         <v>0.0116</v>
       </c>
       <c r="K4" s="8" t="n">
-        <v>0.0179</v>
+        <v>0.0178</v>
       </c>
       <c r="L4" s="8" t="n">
-        <v>0.00938333333333333</v>
+        <v>0.0059</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>0.02815</v>
+        <v>0.0352</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>0.00938333333333333</v>
+        <v>0.00876666666666667</v>
       </c>
       <c r="O4" s="8" t="n">
-        <v>0.00938333333333333</v>
+        <v>0.00876666666666667</v>
       </c>
       <c r="P4" s="8" t="n">
-        <v>0.00938333333333333</v>
+        <v>0.00876666666666667</v>
       </c>
       <c r="Q4" s="8" t="n">
-        <v>0.02815</v>
+        <v>0.0263</v>
       </c>
       <c r="R4" s="8" t="n">
-        <v>0.00938333333333333</v>
+        <v>0.00876666666666667</v>
       </c>
       <c r="S4" s="8" t="n">
-        <v>0.00938333333333333</v>
+        <v>0.00876666666666667</v>
       </c>
       <c r="T4" s="8" t="n">
-        <v>0.00938333333333333</v>
+        <v>0.00876666666666667</v>
       </c>
       <c r="U4" s="8" t="n">
-        <v>0.02815</v>
+        <v>0.0263</v>
       </c>
       <c r="V4" s="8" t="n">
-        <v>0.1126</v>
+        <v>0.1052</v>
       </c>
     </row>
     <row r="5">
@@ -5012,11 +4998,9 @@
       <c r="K7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="L7" s="8" t="n">
-        <v>0.714285714285714</v>
-      </c>
+      <c r="L7" s="8"/>
       <c r="M7" s="8" t="n">
-        <v>0.714285714285714</v>
+        <v>1</v>
       </c>
       <c r="N7" s="8" t="n">
         <v>0.714285714285714</v>
@@ -5139,7 +5123,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="9" t="n">
-        <v>0.0533</v>
+        <v>0.1212</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -5207,7 +5191,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>0.0533</v>
+        <v>0.1212</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -5275,7 +5259,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="9" t="n">
-        <v>0.0533</v>
+        <v>0.1212</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -5299,37 +5283,37 @@
         <v>0</v>
       </c>
       <c r="L4" s="9" t="n">
-        <v>0.0120416666666667</v>
+        <v>0.0625</v>
       </c>
       <c r="M4" s="9" t="n">
-        <v>0.036125</v>
+        <v>0.0599</v>
       </c>
       <c r="N4" s="9" t="n">
-        <v>0.0120416666666667</v>
+        <v>0.0202</v>
       </c>
       <c r="O4" s="9" t="n">
-        <v>0.0120416666666667</v>
+        <v>0.0202</v>
       </c>
       <c r="P4" s="9" t="n">
-        <v>0.0120416666666667</v>
+        <v>0.0202</v>
       </c>
       <c r="Q4" s="9" t="n">
-        <v>0.036125</v>
+        <v>0.0606</v>
       </c>
       <c r="R4" s="9" t="n">
-        <v>0.0120416666666667</v>
+        <v>0.0202</v>
       </c>
       <c r="S4" s="9" t="n">
-        <v>0.0120416666666667</v>
+        <v>0.0202</v>
       </c>
       <c r="T4" s="9" t="n">
-        <v>0.0120416666666667</v>
+        <v>0.0202</v>
       </c>
       <c r="U4" s="9" t="n">
-        <v>0.036125</v>
+        <v>0.0606</v>
       </c>
       <c r="V4" s="9" t="n">
-        <v>0.1445</v>
+        <v>0.2424</v>
       </c>
     </row>
     <row r="5">
@@ -5484,12 +5468,8 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M7" s="9" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
       <c r="N7" s="9" t="n">
         <v>0.5</v>
       </c>

</xml_diff>

<commit_message>
Updated CVDs for the month
</commit_message>
<xml_diff>
--- a/outputs/BURs/BUR Testing_AMC.xlsx
+++ b/outputs/BURs/BUR Testing_AMC.xlsx
@@ -577,7 +577,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.0606</v>
+        <v>0.0634</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -645,7 +645,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0.0606</v>
+        <v>0.0634</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -713,61 +713,61 @@
         <v>24</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.0606</v>
+        <v>0.0634</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.0076</v>
+        <v>0.0075</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0.0115</v>
+        <v>0.0114</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0.0192</v>
+        <v>0.019</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>0.0381</v>
+        <v>0.0378</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>0.0115</v>
+        <v>0.0114</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>0.0038</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.0074</v>
+        <v>0.0073</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.0226</v>
+        <v>0.0224</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>0.0101</v>
+        <v>0.0036</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>0.0101</v>
+        <v>0.00905833333333333</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>0.0101</v>
+        <v>0.00905833333333333</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>0.0303</v>
+        <v>0.027175</v>
       </c>
       <c r="R4" s="1" t="n">
-        <v>0.0101</v>
+        <v>0.00905833333333333</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0.0101</v>
+        <v>0.00905833333333333</v>
       </c>
       <c r="T4" s="1" t="n">
-        <v>0.0101</v>
+        <v>0.00905833333333333</v>
       </c>
       <c r="U4" s="1" t="n">
-        <v>0.0303</v>
+        <v>0.027175</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>0.1212</v>
+        <v>0.1087</v>
       </c>
     </row>
     <row r="5">
@@ -781,7 +781,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -849,7 +849,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -917,7 +917,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -947,31 +947,31 @@
         <v>0.2308</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="R7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="S7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="T7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="U7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="V7" s="1" t="n">
-        <v>0.269230769230769</v>
+        <v>0.233333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -1222,32 +1222,30 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
-      <c r="N4" s="10" t="n">
-        <v>0.0833333333333333</v>
-      </c>
+      <c r="N4" s="10"/>
       <c r="O4" s="10" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.071425</v>
       </c>
       <c r="P4" s="10" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.071425</v>
       </c>
       <c r="Q4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.214275</v>
       </c>
       <c r="R4" s="10" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.071425</v>
       </c>
       <c r="S4" s="10" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.071425</v>
       </c>
       <c r="T4" s="10" t="n">
-        <v>0.0833333333333333</v>
+        <v>0.071425</v>
       </c>
       <c r="U4" s="10" t="n">
-        <v>0.25</v>
+        <v>0.214275</v>
       </c>
       <c r="V4" s="10" t="n">
-        <v>1</v>
+        <v>0.8571</v>
       </c>
     </row>
     <row r="5">
@@ -1463,7 +1461,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="11" t="n">
-        <v>0.0522</v>
+        <v>0.0596</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -1531,7 +1529,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="11" t="n">
-        <v>0.0522</v>
+        <v>0.0596</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -1599,7 +1597,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="11" t="n">
-        <v>0.0522</v>
+        <v>0.0596</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -1614,46 +1612,46 @@
         <v>0.0103</v>
       </c>
       <c r="I4" s="11" t="n">
-        <v>0.0265</v>
+        <v>0.0264</v>
       </c>
       <c r="J4" s="11" t="n">
         <v>0.0099</v>
       </c>
       <c r="K4" s="11" t="n">
-        <v>0.0085</v>
+        <v>0.0084</v>
       </c>
       <c r="L4" s="11" t="n">
-        <v>0.0073</v>
+        <v>0.0076</v>
       </c>
       <c r="M4" s="11" t="n">
-        <v>0.0257</v>
+        <v>0.026</v>
       </c>
       <c r="N4" s="11" t="n">
-        <v>0.0087</v>
+        <v>0.0072</v>
       </c>
       <c r="O4" s="11" t="n">
-        <v>0.0087</v>
+        <v>0.00851666666666667</v>
       </c>
       <c r="P4" s="11" t="n">
-        <v>0.0087</v>
+        <v>0.00851666666666667</v>
       </c>
       <c r="Q4" s="11" t="n">
-        <v>0.0261</v>
+        <v>0.02555</v>
       </c>
       <c r="R4" s="11" t="n">
-        <v>0.0087</v>
+        <v>0.00851666666666667</v>
       </c>
       <c r="S4" s="11" t="n">
-        <v>0.0087</v>
+        <v>0.00851666666666667</v>
       </c>
       <c r="T4" s="11" t="n">
-        <v>0.0087</v>
+        <v>0.00851666666666667</v>
       </c>
       <c r="U4" s="11" t="n">
-        <v>0.0261</v>
+        <v>0.02555</v>
       </c>
       <c r="V4" s="11" t="n">
-        <v>0.1044</v>
+        <v>0.1022</v>
       </c>
     </row>
     <row r="5">
@@ -1667,7 +1665,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1735,7 +1733,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -1803,7 +1801,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -1827,37 +1825,37 @@
         <v>0.6364</v>
       </c>
       <c r="L7" s="11" t="n">
-        <v>0.5385</v>
+        <v>0.625</v>
       </c>
       <c r="M7" s="11" t="n">
-        <v>0.6364</v>
+        <v>0.6552</v>
       </c>
       <c r="N7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.3333</v>
       </c>
       <c r="O7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="P7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="Q7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="R7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="S7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="T7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="U7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
       <c r="V7" s="11" t="n">
-        <v>0.634920634920635</v>
+        <v>0.617021276595745</v>
       </c>
     </row>
   </sheetData>
@@ -1953,7 +1951,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.0081</v>
+        <v>0.008</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2021,7 +2019,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.0081</v>
+        <v>0.008</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2089,7 +2087,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.0081</v>
+        <v>0.008</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -2119,31 +2117,31 @@
         <v>0.008</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0.00135</v>
+        <v>0</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>0.00135</v>
+        <v>0.00114166666666667</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>0.00135</v>
+        <v>0.00114166666666667</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>0.00405</v>
+        <v>0.003425</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>0.00135</v>
+        <v>0.00114166666666667</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>0.00135</v>
+        <v>0.00114166666666667</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>0.00135</v>
+        <v>0.00114166666666667</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>0.00405</v>
+        <v>0.003425</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>0.0162</v>
+        <v>0.0137</v>
       </c>
     </row>
     <row r="5">
@@ -2180,9 +2178,7 @@
       <c r="M5" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="N5" s="2" t="n">
-        <v>0.666666666666667</v>
-      </c>
+      <c r="N5" s="2"/>
       <c r="O5" s="2" t="n">
         <v>0.666666666666667</v>
       </c>
@@ -2301,7 +2297,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.0619</v>
+        <v>0.0675</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -2369,7 +2365,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.0619</v>
+        <v>0.0675</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2437,7 +2433,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.0619</v>
+        <v>0.0675</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -2452,46 +2448,46 @@
         <v>0.0159</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>0.0315</v>
+        <v>0.0316</v>
       </c>
       <c r="J4" s="3" t="n">
         <v>0.0125</v>
       </c>
       <c r="K4" s="3" t="n">
-        <v>0.0071</v>
+        <v>0.0072</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>0.0108</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0.0304</v>
+        <v>0.0305</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>0.0103166666666667</v>
+        <v>0.0054</v>
       </c>
       <c r="O4" s="3" t="n">
-        <v>0.0103166666666667</v>
+        <v>0.00964166666666667</v>
       </c>
       <c r="P4" s="3" t="n">
-        <v>0.0103166666666667</v>
+        <v>0.00964166666666667</v>
       </c>
       <c r="Q4" s="3" t="n">
-        <v>0.03095</v>
+        <v>0.028925</v>
       </c>
       <c r="R4" s="3" t="n">
-        <v>0.0103166666666667</v>
+        <v>0.00964166666666667</v>
       </c>
       <c r="S4" s="3" t="n">
-        <v>0.0103166666666667</v>
+        <v>0.00964166666666667</v>
       </c>
       <c r="T4" s="3" t="n">
-        <v>0.0103166666666667</v>
+        <v>0.00964166666666667</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>0.03095</v>
+        <v>0.028925</v>
       </c>
       <c r="V4" s="3" t="n">
-        <v>0.1238</v>
+        <v>0.1157</v>
       </c>
     </row>
     <row r="5">
@@ -2505,7 +2501,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -2573,7 +2569,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -2641,7 +2637,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -2671,31 +2667,31 @@
         <v>0.7333</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="O7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="P7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="Q7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="R7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="S7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="T7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="U7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
       <c r="V7" s="3" t="n">
-        <v>0.6</v>
+        <v>0.59375</v>
       </c>
     </row>
   </sheetData>
@@ -3181,7 +3177,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.0367</v>
+        <v>0.0469</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3249,7 +3245,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.0367</v>
+        <v>0.0469</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -3317,13 +3313,13 @@
         <v>24</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.0367</v>
+        <v>0.0469</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.0101</v>
+        <v>0.01</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>0.0061</v>
@@ -3332,7 +3328,7 @@
         <v>0.0061</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>0.0223</v>
+        <v>0.0222</v>
       </c>
       <c r="J4" s="5" t="n">
         <v>0.0082</v>
@@ -3344,34 +3340,34 @@
         <v>0.002</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>0.0144</v>
+        <v>0.0143</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>0.00611666666666667</v>
+        <v>0.0102</v>
       </c>
       <c r="O4" s="5" t="n">
-        <v>0.00611666666666667</v>
+        <v>0.0067</v>
       </c>
       <c r="P4" s="5" t="n">
-        <v>0.00611666666666667</v>
+        <v>0.0067</v>
       </c>
       <c r="Q4" s="5" t="n">
-        <v>0.01835</v>
+        <v>0.0201</v>
       </c>
       <c r="R4" s="5" t="n">
-        <v>0.00611666666666667</v>
+        <v>0.0067</v>
       </c>
       <c r="S4" s="5" t="n">
-        <v>0.00611666666666667</v>
+        <v>0.0067</v>
       </c>
       <c r="T4" s="5" t="n">
-        <v>0.00611666666666667</v>
+        <v>0.0067</v>
       </c>
       <c r="U4" s="5" t="n">
-        <v>0.01835</v>
+        <v>0.0201</v>
       </c>
       <c r="V4" s="5" t="n">
-        <v>0.0734</v>
+        <v>0.0804</v>
       </c>
     </row>
     <row r="5">
@@ -3385,7 +3381,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -3453,7 +3449,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -3521,7 +3517,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -3551,31 +3547,31 @@
         <v>0.6667</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0</v>
       </c>
       <c r="O7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="P7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="Q7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="R7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="S7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="T7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="U7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="V7" s="5" t="n">
-        <v>0.761904761904762</v>
+        <v>0.666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -3671,7 +3667,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>0.031</v>
+        <v>0.0369</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -3739,7 +3735,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>0.031</v>
+        <v>0.0369</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -3807,7 +3803,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>0.031</v>
+        <v>0.0369</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -3822,7 +3818,7 @@
         <v>0.0084</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>0.0139</v>
+        <v>0.014</v>
       </c>
       <c r="J4" s="6" t="n">
         <v>0.0085</v>
@@ -3834,34 +3830,34 @@
         <v>0.0029</v>
       </c>
       <c r="M4" s="6" t="n">
-        <v>0.0171</v>
+        <v>0.0172</v>
       </c>
       <c r="N4" s="6" t="n">
-        <v>0.00516666666666667</v>
+        <v>0.0058</v>
       </c>
       <c r="O4" s="6" t="n">
-        <v>0.00516666666666667</v>
+        <v>0.005275</v>
       </c>
       <c r="P4" s="6" t="n">
-        <v>0.00516666666666667</v>
+        <v>0.005275</v>
       </c>
       <c r="Q4" s="6" t="n">
-        <v>0.0155</v>
+        <v>0.015825</v>
       </c>
       <c r="R4" s="6" t="n">
-        <v>0.00516666666666667</v>
+        <v>0.005275</v>
       </c>
       <c r="S4" s="6" t="n">
-        <v>0.00516666666666667</v>
+        <v>0.005275</v>
       </c>
       <c r="T4" s="6" t="n">
-        <v>0.00516666666666667</v>
+        <v>0.005275</v>
       </c>
       <c r="U4" s="6" t="n">
-        <v>0.0155</v>
+        <v>0.015825</v>
       </c>
       <c r="V4" s="6" t="n">
-        <v>0.062</v>
+        <v>0.0633</v>
       </c>
     </row>
     <row r="5">
@@ -4036,9 +4032,7 @@
       <c r="M7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="N7" s="6" t="n">
-        <v>0.888888888888889</v>
-      </c>
+      <c r="N7" s="6"/>
       <c r="O7" s="6" t="n">
         <v>0.888888888888889</v>
       </c>
@@ -4157,7 +4151,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>0.0647</v>
+        <v>0.0734</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -4225,7 +4219,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>0.0647</v>
+        <v>0.0734</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -4293,61 +4287,61 @@
         <v>24</v>
       </c>
       <c r="D4" s="7" t="n">
-        <v>0.0647</v>
+        <v>0.0734</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
       </c>
       <c r="F4" s="7" t="n">
-        <v>0.0139</v>
+        <v>0.0137</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>0.0079</v>
+        <v>0.0078</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>0.0063</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>0.0282</v>
+        <v>0.0279</v>
       </c>
       <c r="J4" s="7" t="n">
-        <v>0.0094</v>
+        <v>0.0093</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>0.0159</v>
+        <v>0.0157</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>0.0112</v>
+        <v>0.0127</v>
       </c>
       <c r="M4" s="7" t="n">
-        <v>0.0365</v>
+        <v>0.0377</v>
       </c>
       <c r="N4" s="7" t="n">
-        <v>0.0107833333333333</v>
+        <v>0.0079</v>
       </c>
       <c r="O4" s="7" t="n">
-        <v>0.0107833333333333</v>
+        <v>0.0104833333333333</v>
       </c>
       <c r="P4" s="7" t="n">
-        <v>0.0107833333333333</v>
+        <v>0.0104833333333333</v>
       </c>
       <c r="Q4" s="7" t="n">
-        <v>0.03235</v>
+        <v>0.03145</v>
       </c>
       <c r="R4" s="7" t="n">
-        <v>0.0107833333333333</v>
+        <v>0.0104833333333333</v>
       </c>
       <c r="S4" s="7" t="n">
-        <v>0.0107833333333333</v>
+        <v>0.0104833333333333</v>
       </c>
       <c r="T4" s="7" t="n">
-        <v>0.0107833333333333</v>
+        <v>0.0104833333333333</v>
       </c>
       <c r="U4" s="7" t="n">
-        <v>0.03235</v>
+        <v>0.03145</v>
       </c>
       <c r="V4" s="7" t="n">
-        <v>0.1294</v>
+        <v>0.1258</v>
       </c>
     </row>
     <row r="5">
@@ -4361,7 +4355,7 @@
         <v>28</v>
       </c>
       <c r="D5" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -4427,7 +4421,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -4495,7 +4489,7 @@
         <v>28</v>
       </c>
       <c r="D7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="E7" t="s">
         <v>27</v>
@@ -4519,37 +4513,37 @@
         <v>1</v>
       </c>
       <c r="L7" s="7" t="n">
-        <v>0.75</v>
+        <v>0.8571</v>
       </c>
       <c r="M7" s="7" t="n">
-        <v>0.8333</v>
+        <v>0.8667</v>
       </c>
       <c r="N7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>1</v>
       </c>
       <c r="O7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="P7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="Q7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="R7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="S7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="T7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="U7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
       <c r="V7" s="7" t="n">
-        <v>0.846153846153846</v>
+        <v>0.875</v>
       </c>
     </row>
   </sheetData>
@@ -4645,7 +4639,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="8" t="n">
-        <v>0.0526</v>
+        <v>0.0701</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -4713,7 +4707,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="8" t="n">
-        <v>0.0526</v>
+        <v>0.0701</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -4781,7 +4775,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="8" t="n">
-        <v>0.0526</v>
+        <v>0.0701</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -4796,46 +4790,46 @@
         <v>0</v>
       </c>
       <c r="I4" s="8" t="n">
-        <v>0.0175</v>
+        <v>0.0174</v>
       </c>
       <c r="J4" s="8" t="n">
-        <v>0.0116</v>
+        <v>0.0115</v>
       </c>
       <c r="K4" s="8" t="n">
-        <v>0.0178</v>
+        <v>0.0176</v>
       </c>
       <c r="L4" s="8" t="n">
         <v>0.0059</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>0.0352</v>
+        <v>0.035</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>0.00876666666666667</v>
+        <v>0.018</v>
       </c>
       <c r="O4" s="8" t="n">
-        <v>0.00876666666666667</v>
+        <v>0.0100166666666667</v>
       </c>
       <c r="P4" s="8" t="n">
-        <v>0.00876666666666667</v>
+        <v>0.0100166666666667</v>
       </c>
       <c r="Q4" s="8" t="n">
-        <v>0.0263</v>
+        <v>0.03005</v>
       </c>
       <c r="R4" s="8" t="n">
-        <v>0.00876666666666667</v>
+        <v>0.0100166666666667</v>
       </c>
       <c r="S4" s="8" t="n">
-        <v>0.00876666666666667</v>
+        <v>0.0100166666666667</v>
       </c>
       <c r="T4" s="8" t="n">
-        <v>0.00876666666666667</v>
+        <v>0.0100166666666667</v>
       </c>
       <c r="U4" s="8" t="n">
-        <v>0.0263</v>
+        <v>0.03005</v>
       </c>
       <c r="V4" s="8" t="n">
-        <v>0.1052</v>
+        <v>0.1202</v>
       </c>
     </row>
     <row r="5">
@@ -5002,9 +4996,7 @@
       <c r="M7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="N7" s="8" t="n">
-        <v>0.714285714285714</v>
-      </c>
+      <c r="N7" s="8"/>
       <c r="O7" s="8" t="n">
         <v>0.714285714285714</v>
       </c>
@@ -5123,7 +5115,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="9" t="n">
-        <v>0.1212</v>
+        <v>0.1205</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -5191,7 +5183,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>0.1212</v>
+        <v>0.1205</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -5259,7 +5251,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="9" t="n">
-        <v>0.1212</v>
+        <v>0.1205</v>
       </c>
       <c r="E4" t="s">
         <v>27</v>
@@ -5289,31 +5281,31 @@
         <v>0.0599</v>
       </c>
       <c r="N4" s="9" t="n">
-        <v>0.0202</v>
+        <v>0</v>
       </c>
       <c r="O4" s="9" t="n">
-        <v>0.0202</v>
+        <v>0.0172166666666667</v>
       </c>
       <c r="P4" s="9" t="n">
-        <v>0.0202</v>
+        <v>0.0172166666666667</v>
       </c>
       <c r="Q4" s="9" t="n">
-        <v>0.0606</v>
+        <v>0.05165</v>
       </c>
       <c r="R4" s="9" t="n">
-        <v>0.0202</v>
+        <v>0.0172166666666667</v>
       </c>
       <c r="S4" s="9" t="n">
-        <v>0.0202</v>
+        <v>0.0172166666666667</v>
       </c>
       <c r="T4" s="9" t="n">
-        <v>0.0202</v>
+        <v>0.0172166666666667</v>
       </c>
       <c r="U4" s="9" t="n">
-        <v>0.0606</v>
+        <v>0.05165</v>
       </c>
       <c r="V4" s="9" t="n">
-        <v>0.2424</v>
+        <v>0.2066</v>
       </c>
     </row>
     <row r="5">
@@ -5470,9 +5462,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="9" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="N7" s="9"/>
       <c r="O7" s="9" t="n">
         <v>0.5</v>
       </c>

</xml_diff>